<commit_message>
Accuracy and Excel Updated
</commit_message>
<xml_diff>
--- a/testXL.xlsx
+++ b/testXL.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="22960" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="3500" yWindow="0" windowWidth="15920" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,62 +19,181 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>happy</t>
   </si>
   <si>
-    <t>happy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>happy_1.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>happy_2.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>neutral_1.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>neutral_2.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>fishy</t>
+  </si>
+  <si>
+    <t>surprised</t>
+  </si>
+  <si>
+    <t>angry</t>
   </si>
   <si>
     <t>neutral</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>neutral</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>happy_3.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>happy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2013-11-09 17.11.29.jog</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.11.50.jog</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.13.18.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.13.34.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.13.52.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.13.55.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.13.58.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.14.02.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.14.06.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.14.25.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.15.27.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.15.30.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.15.53.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.16.07.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.16.17.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.17.20.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.18.20.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.18.22.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.18.25.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.18.28.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.18.49.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.19.37.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.19.47.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.19.49.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.19.55.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.19.58.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.20.07.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.20.15.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.20.16.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.20.46.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.20.58.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.32.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.34.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.37.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.40.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.42.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.43.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.45.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.46.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.47</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.56.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.21.58.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.03.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.04.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.06.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.07.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.09.jpg</t>
+  </si>
+  <si>
+    <t>2013-11-09 17.22.22.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +223,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -429,60 +548,432 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>